<commit_message>
read/write functional without units
</commit_message>
<xml_diff>
--- a/Sub_Output.xlsx
+++ b/Sub_Output.xlsx
@@ -26,13 +26,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -51,12 +56,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -85,12 +105,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -551,17 +574,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>value</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>units</t>
         </is>
@@ -593,7 +616,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>km/h</t>
+          <t>m/s</t>
         </is>
       </c>
     </row>
@@ -608,7 +631,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>rad</t>
+          <t>sec</t>
         </is>
       </c>
     </row>
@@ -623,7 +646,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sec</t>
+          <t>kg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
AOCS very rough estimates
</commit_message>
<xml_diff>
--- a/Sub_Output.xlsx
+++ b/Sub_Output.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
   <si>
     <t>name</t>
   </si>
@@ -91,7 +91,52 @@
     <t>current type</t>
   </si>
   <si>
-    <t>AC or DC</t>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>P RCS fuel</t>
+  </si>
+  <si>
+    <t>O RCS fuel</t>
+  </si>
+  <si>
+    <t>P dry mass</t>
+  </si>
+  <si>
+    <t>probe AOCS dry mass</t>
+  </si>
+  <si>
+    <t>O dry mass</t>
+  </si>
+  <si>
+    <t>orbiter AOCS dry mass</t>
+  </si>
+  <si>
+    <t>tbd</t>
+  </si>
+  <si>
+    <t>P min power</t>
+  </si>
+  <si>
+    <t>probe min power</t>
+  </si>
+  <si>
+    <t>probe max power</t>
+  </si>
+  <si>
+    <t>orbiter max power</t>
+  </si>
+  <si>
+    <t>O min power</t>
+  </si>
+  <si>
+    <t>orbiter min power</t>
+  </si>
+  <si>
+    <t>AC vs DC</t>
+  </si>
+  <si>
+    <t>orbiter, may use thrusters from propulsion system</t>
   </si>
 </sst>
 </file>
@@ -110,11 +155,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -601,15 +648,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,6 +678,9 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -641,6 +692,9 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
@@ -652,6 +706,9 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
@@ -663,6 +720,9 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -672,10 +732,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
@@ -683,24 +746,111 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>333</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>102</v>
+      </c>
+      <c r="C14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moment of inertia function added to definitions, AOCS end-of-day budget (no)update
</commit_message>
<xml_diff>
--- a/Sub_Output.xlsx
+++ b/Sub_Output.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexisPC\PycharmProjects\DSE-Mars-Reveal\project\subsystems_design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lmaio\Nextcloud\TU Delft\2019-2020\DSE-Mars-Reveal\project\subsystems_design\AOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E6ECC7-9BAC-442F-A8D1-D11F78B2A8DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="1830" windowWidth="20370" windowHeight="13020" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1245" yWindow="1830" windowWidth="20370" windowHeight="13020" tabRatio="719" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="EPS" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
     <sheet name="Astro" sheetId="10" r:id="rId10"/>
     <sheet name="AOCS" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="197">
   <si>
     <t>name</t>
   </si>
@@ -625,12 +624,18 @@
   </si>
   <si>
     <t>degrees</t>
+  </si>
+  <si>
+    <t>max_pt_excur</t>
+  </si>
+  <si>
+    <t>Maximum pointing excursion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1055,11 +1060,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A20" sqref="A20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,13 +1341,27 @@
         <v>132</v>
       </c>
     </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B20">
+        <v>23.5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1490,7 +1509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1703,15 +1722,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1867,13 +1887,27 @@
         <v>66</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B12">
+        <v>42.4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1882,7 +1916,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1914,7 +1949,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2010,10 +2045,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -2361,11 +2396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,7 +2601,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2715,10 +2750,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2745,7 +2780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
end of day budgets, fixed atmos prop
</commit_message>
<xml_diff>
--- a/Sub_Output.xlsx
+++ b/Sub_Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="9" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="750" visibility="visible" windowHeight="13020" windowWidth="20370" xWindow="2865" yWindow="1830"/>
+    <workbookView activeTab="8" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="750" visibility="visible" windowHeight="13020" windowWidth="20370" xWindow="2865" yWindow="1830"/>
   </bookViews>
   <sheets>
     <sheet name="EPS" sheetId="1" state="visible" r:id="rId1"/>
@@ -33,12 +33,6 @@
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -83,6 +77,12 @@
       <sz val="11"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -94,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -183,6 +183,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -198,26 +213,23 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -226,10 +238,13 @@
     <xf applyAlignment="1" borderId="5" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="7" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="8" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="9" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -939,7 +954,7 @@
           <t>dimension</t>
         </is>
       </c>
-      <c r="B20" s="10" t="inlineStr">
+      <c r="B20" s="9" t="inlineStr">
         <is>
           <t>245.6 x 213.4 x 165.5'</t>
         </is>
@@ -956,7 +971,7 @@
           <t>dim_pcdu</t>
         </is>
       </c>
-      <c r="B21" s="11" t="inlineStr">
+      <c r="B21" s="10" t="inlineStr">
         <is>
           <t>"0.348*0.17*0.222"</t>
         </is>
@@ -1010,22 +1025,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="14" t="inlineStr">
+      <c r="A1" s="13" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="14" t="inlineStr">
+      <c r="B1" s="13" t="inlineStr">
         <is>
           <t>value</t>
         </is>
       </c>
-      <c r="C1" s="14" t="inlineStr">
+      <c r="C1" s="13" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
       </c>
-      <c r="D1" s="14" t="inlineStr">
+      <c r="D1" s="13" t="inlineStr">
         <is>
           <t>units</t>
         </is>
@@ -1954,7 +1969,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1975,12 +1990,12 @@
       </c>
       <c r="C1" s="15" t="inlineStr">
         <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="D1" s="15" t="inlineStr">
+        <is>
           <t>description</t>
-        </is>
-      </c>
-      <c r="D1" s="15" t="inlineStr">
-        <is>
-          <t>units</t>
         </is>
       </c>
     </row>
@@ -1997,12 +2012,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>probe</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>C</t>
         </is>
       </c>
     </row>
@@ -2019,12 +2034,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>probe</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>C</t>
         </is>
       </c>
     </row>
@@ -2041,12 +2056,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>orbiter</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>C</t>
         </is>
       </c>
     </row>
@@ -2063,12 +2078,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>orbiter</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>C</t>
         </is>
       </c>
     </row>
@@ -2083,12 +2098,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>probe min power</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>W</t>
         </is>
       </c>
     </row>
@@ -2103,12 +2118,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>probe max power</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>W</t>
         </is>
       </c>
     </row>
@@ -2123,12 +2138,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>W</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>orbiter min power</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>W</t>
         </is>
       </c>
     </row>
@@ -2143,12 +2158,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t xml:space="preserve">W </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>orbiter max power</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">W </t>
         </is>
       </c>
     </row>
@@ -2163,12 +2178,12 @@
           <t>tbd</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
         <is>
           <t>AC vs DC</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2181,12 +2196,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>probe</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>kg</t>
         </is>
       </c>
     </row>
@@ -2203,12 +2218,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>orbiter, may use thrusters from propulsion system</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>kg</t>
         </is>
       </c>
     </row>
@@ -2223,12 +2238,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>probe AOCS dry mass</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>kg</t>
         </is>
       </c>
     </row>
@@ -2243,12 +2258,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>orbiter AOCS dry mass</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>kg</t>
         </is>
       </c>
     </row>
@@ -2259,9 +2274,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.3240003977512775</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
+        <v>5.136607233021042e-06</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>N m</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
@@ -2271,24 +2290,62 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>2115.497182307744</v>
-      </c>
-      <c r="C16" t="inlineStr"/>
+        <v>0.01235472322116449</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>N m s</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>orb_max_disturb_name</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>aerodynamic</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
+          <t>aero drag</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1.06466552853985e-11</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>orb_max_disturb_type</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>solar</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ignored mass bodies</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>bodies ignored for aerodynamic calculations</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -2725,22 +2782,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="inlineStr">
+      <c r="A1" s="11" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="12" t="inlineStr">
+      <c r="B1" s="11" t="inlineStr">
         <is>
           <t>value</t>
         </is>
       </c>
-      <c r="C1" s="12" t="inlineStr">
+      <c r="C1" s="11" t="inlineStr">
         <is>
           <t>units</t>
         </is>
       </c>
-      <c r="E1" s="13" t="inlineStr">
+      <c r="E1" s="12" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
@@ -3658,12 +3715,12 @@
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="2" thickBot="1">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>D</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="2" t="n">
         <v>1.5</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -3678,12 +3735,12 @@
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="3" thickBot="1">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>l</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
+      <c r="B3" s="2" t="n">
         <v>1.8</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -3706,22 +3763,22 @@
           <t xml:space="preserve">MW/m^2 </t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">from Viking mission that had a higher velocity while entring the mars atmosphere </t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="5" thickBot="1">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>a_entry</t>
         </is>
       </c>
-      <c r="B5" s="3" t="n">
+      <c r="B5" s="2" t="n">
         <v>60</v>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>m/s^2</t>
         </is>
@@ -3733,15 +3790,15 @@
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="6" thickBot="1">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>dynamic_press</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B6" s="2" t="n">
         <v>500</v>
       </c>
-      <c r="C6" s="3" t="n"/>
+      <c r="C6" s="2" t="n"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>phoenix - 2001 mars (500-625)</t>
@@ -3749,15 +3806,15 @@
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="7" thickBot="1">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>altitude</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>km</t>
         </is>
@@ -3769,15 +3826,15 @@
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="8" thickBot="1">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>M_para</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="2" t="n">
         <v>1.3</v>
       </c>
-      <c r="C8" s="3" t="n"/>
+      <c r="C8" s="2" t="n"/>
       <c r="D8" t="inlineStr">
         <is>
           <t>Mach number for  parachute deployment (1.1- 1.6)</t>
@@ -3785,15 +3842,15 @@
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="9" thickBot="1">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Cd_para</t>
         </is>
       </c>
-      <c r="B9" s="3" t="n">
+      <c r="B9" s="2" t="n">
         <v>0.3</v>
       </c>
-      <c r="C9" s="3" t="n"/>
+      <c r="C9" s="2" t="n"/>
       <c r="D9" t="inlineStr">
         <is>
           <t>Cd for parachutes (0.3-0.6)</t>
@@ -3801,22 +3858,22 @@
       </c>
     </row>
     <row customHeight="1" ht="15.75" r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>H</t>
         </is>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="7" t="n">
         <v>11.1</v>
       </c>
-      <c r="D10" s="9" t="inlineStr">
+      <c r="D10" s="8" t="inlineStr">
         <is>
           <t>Scale height</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5" t="inlineStr">
+      <c r="A11" s="4" t="inlineStr">
         <is>
           <t>dv_thrust</t>
         </is>
@@ -3836,12 +3893,12 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="inlineStr">
+      <c r="A12" s="4" t="inlineStr">
         <is>
           <t>alt_thrust</t>
         </is>
       </c>
-      <c r="B12" s="5" t="n">
+      <c r="B12" s="4" t="n">
         <v>900</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -3898,7 +3955,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>V_HP3_WEM</t>
         </is>
@@ -3918,7 +3975,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="inlineStr">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>ground_clearance</t>
         </is>
@@ -3938,7 +3995,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="6" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>f_max_sampling</t>
         </is>
@@ -3958,7 +4015,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="6" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>max_inclination</t>
         </is>
@@ -3978,7 +4035,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="inlineStr">
+      <c r="A6" s="5" t="inlineStr">
         <is>
           <t>seis_dome_mass</t>
         </is>
@@ -3998,7 +4055,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="inlineStr">
+      <c r="A7" s="5" t="inlineStr">
         <is>
           <t>seis_dome_diam</t>
         </is>
@@ -4018,7 +4075,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="6" t="inlineStr">
+      <c r="A8" s="5" t="inlineStr">
         <is>
           <t>seis_dome_height</t>
         </is>
@@ -4038,7 +4095,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="inlineStr">
+      <c r="A9" s="5" t="inlineStr">
         <is>
           <t>windshield_mass</t>
         </is>
@@ -4125,8 +4182,8 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -4160,7 +4217,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -4469,7 +4526,7 @@
           <t>max ballistic coeff</t>
         </is>
       </c>
-      <c r="B20" s="7" t="n">
+      <c r="B20" s="6" t="n">
         <v>164.2125</v>
       </c>
       <c r="D20" t="inlineStr">
@@ -4484,7 +4541,7 @@
           <t>min ballistic coeff</t>
         </is>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="6" t="n">
         <v>33.2625</v>
       </c>
       <c r="D21" t="inlineStr">

</xml_diff>

<commit_message>
AOCS sizing model complete
</commit_message>
<xml_diff>
--- a/Sub_Output.xlsx
+++ b/Sub_Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="8" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="750" visibility="visible" windowHeight="13020" windowWidth="20370" xWindow="2865" yWindow="1830"/>
+    <workbookView activeTab="10" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="750" visibility="visible" windowHeight="13020" windowWidth="20370" xWindow="2865" yWindow="1830"/>
   </bookViews>
   <sheets>
     <sheet name="EPS" sheetId="1" state="visible" r:id="rId1"/>
@@ -78,7 +78,6 @@
     </font>
     <font>
       <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -1016,7 +1015,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -1969,7 +1968,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1990,12 +1989,12 @@
       </c>
       <c r="C1" s="15" t="inlineStr">
         <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="D1" s="15" t="inlineStr">
+        <is>
           <t>units</t>
-        </is>
-      </c>
-      <c r="D1" s="15" t="inlineStr">
-        <is>
-          <t>description</t>
         </is>
       </c>
     </row>
@@ -2012,12 +2011,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>probe</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>C</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>probe</t>
         </is>
       </c>
     </row>
@@ -2034,12 +2033,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>probe</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>C</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>probe</t>
         </is>
       </c>
     </row>
@@ -2056,12 +2055,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>orbiter</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>C</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>orbiter</t>
         </is>
       </c>
     </row>
@@ -2078,12 +2077,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>orbiter</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>C</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>orbiter</t>
         </is>
       </c>
     </row>
@@ -2098,12 +2097,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>probe min power</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>W</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>probe min power</t>
         </is>
       </c>
     </row>
@@ -2118,12 +2117,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>probe max power</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>W</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>probe max power</t>
         </is>
       </c>
     </row>
@@ -2138,12 +2137,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>orbiter min power</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>W</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>orbiter min power</t>
         </is>
       </c>
     </row>
@@ -2158,12 +2157,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>orbiter max power</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t xml:space="preserve">W </t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>orbiter max power</t>
         </is>
       </c>
     </row>
@@ -2178,12 +2177,12 @@
           <t>tbd</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>AC vs DC</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2196,12 +2195,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>probe</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>kg</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>probe</t>
         </is>
       </c>
     </row>
@@ -2211,19 +2210,17 @@
           <t>O RCS fuel</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>tbd</t>
-        </is>
+      <c r="B12" t="n">
+        <v>0.01234936006686301</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>orbiter, may use thrusters from propulsion system</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>kg</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>orbiter, may use thrusters from propulsion system</t>
         </is>
       </c>
     </row>
@@ -2238,12 +2235,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>probe AOCS dry mass</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>kg</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>probe AOCS dry mass</t>
         </is>
       </c>
     </row>
@@ -2258,12 +2255,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>orbiter AOCS dry mass</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>kg</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>orbiter AOCS dry mass</t>
         </is>
       </c>
     </row>
@@ -2274,14 +2271,14 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>5.136607233021042e-06</v>
-      </c>
-      <c r="C15" t="inlineStr">
+        <v>5.191050069557283e-06</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
         <is>
           <t>N m</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2290,14 +2287,14 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01235472322116449</v>
-      </c>
-      <c r="C16" t="inlineStr">
+        <v>0.01158319792854069</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr">
         <is>
           <t>N m s</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2306,14 +2303,14 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.06466552853985e-11</v>
-      </c>
-      <c r="C17" t="inlineStr">
+        <v>3.099910352992988e-06</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr">
         <is>
           <t>N</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2340,10 +2337,54 @@
           <t>[]</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>bodies ignored for aerodynamic calculations</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>thruster pulses</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>5481</v>
+      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>min thrust momentum dump</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2.80880410134032e-06</v>
+      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>min thrust slew</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0.03025937608330904</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>
@@ -4182,8 +4223,8 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -4217,7 +4258,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Model fully working, all hardware design choices available
</commit_message>
<xml_diff>
--- a/Sub_Output.xlsx
+++ b/Sub_Output.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="341">
   <si>
     <t>name</t>
   </si>
@@ -955,12 +955,12 @@
     <t>P min temp</t>
   </si>
   <si>
+    <t>probe</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
-    <t>probe</t>
-  </si>
-  <si>
     <t>P max temp</t>
   </si>
   <si>
@@ -994,12 +994,12 @@
     <t>O max power</t>
   </si>
   <si>
+    <t>orbiter max power</t>
+  </si>
+  <si>
     <t xml:space="preserve">W </t>
   </si>
   <si>
-    <t>orbiter max power</t>
-  </si>
-  <si>
     <t>current type</t>
   </si>
   <si>
@@ -1039,10 +1039,19 @@
     <t>O avg_power</t>
   </si>
   <si>
-    <t>P mass</t>
-  </si>
-  <si>
-    <t>P volume</t>
+    <t>P mass w/ HS</t>
+  </si>
+  <si>
+    <t>P volume w/ HS</t>
+  </si>
+  <si>
+    <t>P mass lander</t>
+  </si>
+  <si>
+    <t>P volume lander</t>
+  </si>
+  <si>
+    <t>P power lander</t>
   </si>
 </sst>
 </file>
@@ -1103,6 +1112,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2583,11 +2593,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="14" t="s">
@@ -2597,10 +2612,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2639,10 +2654,10 @@
         <v>-30</v>
       </c>
       <c r="C4" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2653,10 +2668,10 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2667,10 +2682,10 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D6" t="s">
         <v>91</v>
-      </c>
-      <c r="D6" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2681,10 +2696,10 @@
         <v>200</v>
       </c>
       <c r="C7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D7" t="s">
         <v>91</v>
-      </c>
-      <c r="D7" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2695,10 +2710,10 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" t="s">
         <v>91</v>
-      </c>
-      <c r="D8" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2722,7 +2737,7 @@
       <c r="B10" t="s">
         <v>324</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" t="s">
         <v>325</v>
       </c>
     </row>
@@ -2734,10 +2749,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>308</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
-      </c>
-      <c r="D11" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2748,10 +2763,10 @@
         <v>4.8173104512163618E-2</v>
       </c>
       <c r="C12" t="s">
+        <v>328</v>
+      </c>
+      <c r="D12" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2762,10 +2777,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>330</v>
+      </c>
+      <c r="D13" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2776,10 +2791,10 @@
         <v>102</v>
       </c>
       <c r="C14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2811,7 +2826,7 @@
         <v>336</v>
       </c>
       <c r="B18">
-        <v>3.37365</v>
+        <v>3.37</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2819,7 +2834,31 @@
         <v>337</v>
       </c>
       <c r="B19">
-        <v>4.1392999999999999E-2</v>
+        <v>1.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>338</v>
+      </c>
+      <c r="B20">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>339</v>
+      </c>
+      <c r="B21">
+        <v>0.31759999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>340</v>
+      </c>
+      <c r="B22">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -4170,12 +4209,12 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
     <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
AOCS main file added
</commit_message>
<xml_diff>
--- a/Sub_Output.xlsx
+++ b/Sub_Output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="10" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="761" visibility="visible" windowHeight="13020" windowWidth="20370" xWindow="5010" yWindow="1425"/>
+    <workbookView activeTab="10" autoFilterDateGrouping="1" firstSheet="0" minimized="1" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="761" visibility="visible" windowHeight="13020" windowWidth="20370" xWindow="5010" yWindow="1425"/>
   </bookViews>
   <sheets>
     <sheet name="EPS" sheetId="1" state="visible" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="AOCS" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1801,7 +1801,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>34.4</v>
+        <v>13.91</v>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>

</xml_diff>